<commit_message>
Testes realizados - Versão completa
</commit_message>
<xml_diff>
--- a/nome_email_bibliotecas.xlsx
+++ b/nome_email_bibliotecas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudprodamazhotmail-my.sharepoint.com/personal/joaovpires_prefeitura_sp_gov_br/Documents/Documentos/AutomacaoQuedaRede/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x540865\Documents\AutomacaoQuedaRede\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_D64A3CD197D9AECF8A160B3DCB361B6479B003E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E94D4988-A0A1-41EE-AA7F-72B41D6AD1A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30CE677-DC71-47F6-B7E1-056276C22523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Nome</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Biblioteca Cassiano Ricardo</t>
   </si>
   <si>
-    <t>BIBLIOTECA ÉRICO VERÍSSIMO</t>
-  </si>
-  <si>
     <t>Biblioteca Pe. José Anchieta</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Biblioteca Paulo Setúbal</t>
   </si>
   <si>
-    <t>BIBLIOTECA SYLVIA ORTHOF</t>
-  </si>
-  <si>
     <t>Biblioteca Alceu Amoroso Lima</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>Biblioteca Raimundo de Menezes</t>
   </si>
   <si>
-    <t>BIBLIOTECA ÁLVARO GUERRA</t>
-  </si>
-  <si>
     <t>Biblioteca Prof. Arnaldo M. Giácomo</t>
   </si>
   <si>
@@ -377,6 +368,21 @@
   </si>
   <si>
     <t>jveloso4669@gmail.com</t>
+  </si>
+  <si>
+    <t>caue.ms04@gmail.com</t>
+  </si>
+  <si>
+    <t>Biblioteca Érico Veríssimo</t>
+  </si>
+  <si>
+    <t>Biblioteca Sylvia Orthof</t>
+  </si>
+  <si>
+    <t>Biblioteca Álvaro Guerra</t>
+  </si>
+  <si>
+    <t>espaguetecomalmondega00@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -757,14 +763,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +835,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -836,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,7 +851,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +859,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -860,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -868,384 +875,395 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>92</v>
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>93</v>
+        <v>119</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B43" r:id="rId1" xr:uid="{CEF77893-9250-4821-8E5F-DBD435BF7A80}"/>
+    <hyperlink ref="B34" r:id="rId2" xr:uid="{6D7991AB-4BD9-44E0-8F79-8E0F14FF3A4C}"/>
+    <hyperlink ref="B35" r:id="rId3" xr:uid="{B8EDB480-70A7-41E7-9D04-51D0C0D4E294}"/>
+    <hyperlink ref="B24" r:id="rId4" xr:uid="{7D2703FC-085D-4E32-B0A5-2546CC1E0251}"/>
+    <hyperlink ref="C24" r:id="rId5" xr:uid="{FE0AAD90-97D8-40C6-ADEE-4B95FD4558FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>